<commit_message>
Started reading excel file
</commit_message>
<xml_diff>
--- a/Testing/Klassenbildung Testdatei LoL.xlsx
+++ b/Testing/Klassenbildung Testdatei LoL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanni\Documents\Arbeit\Kanton St. Gallen\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B018EFF-F5AA-42D8-A479-4BBCBEE112A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041A1AB6-38DB-44A2-B86D-2B3AE73EEDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="84">
   <si>
     <t>id</t>
   </si>
@@ -150,6 +150,129 @@
   <si>
     <t>Bard</t>
   </si>
+  <si>
+    <t>Cassandra</t>
+  </si>
+  <si>
+    <t>Ximena</t>
+  </si>
+  <si>
+    <t>Mayym</t>
+  </si>
+  <si>
+    <t>O-ma</t>
+  </si>
+  <si>
+    <t>Du Couteau</t>
+  </si>
+  <si>
+    <t>Katarina</t>
+  </si>
+  <si>
+    <t>Marcus</t>
+  </si>
+  <si>
+    <t>Soreana</t>
+  </si>
+  <si>
+    <t>Tobias</t>
+  </si>
+  <si>
+    <t>Familie</t>
+  </si>
+  <si>
+    <t>Sentinel</t>
+  </si>
+  <si>
+    <t>Bridge of Progress 1</t>
+  </si>
+  <si>
+    <t>Bridge of Progress 2</t>
+  </si>
+  <si>
+    <t>Bridge of Progress 3</t>
+  </si>
+  <si>
+    <t>Piltover</t>
+  </si>
+  <si>
+    <t>The Last Drop</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Immortal Bastion Alley 1</t>
+  </si>
+  <si>
+    <t>Noxus</t>
+  </si>
+  <si>
+    <t>Placidium</t>
+  </si>
+  <si>
+    <t>Ionia</t>
+  </si>
+  <si>
+    <t>The Lands</t>
+  </si>
+  <si>
+    <t>Queens Palace</t>
+  </si>
+  <si>
+    <t>Ixtal</t>
+  </si>
+  <si>
+    <t>Immortal Bastion Alley 2</t>
+  </si>
+  <si>
+    <t>Wirtschaft und Recht</t>
+  </si>
+  <si>
+    <t>Spanisch</t>
+  </si>
+  <si>
+    <t>Biologie und Chemie</t>
+  </si>
+  <si>
+    <t>Italienisch</t>
+  </si>
+  <si>
+    <t>Physik und Anwendungen der Mathematik</t>
+  </si>
+  <si>
+    <t>deutsch</t>
+  </si>
+  <si>
+    <t>zweisprachig</t>
+  </si>
+  <si>
+    <t>Biologie und Chemie mit IB</t>
+  </si>
+  <si>
+    <t>Bildnerisches Gestalten</t>
+  </si>
+  <si>
+    <t>Physik und Anwendungen der Mathematik mit IB</t>
+  </si>
+  <si>
+    <t>Kantonsschule Heerbrugg</t>
+  </si>
+  <si>
+    <t>Kantonsschule am Burggraben St.Gallen</t>
+  </si>
+  <si>
+    <t>Kantonsschule Wil</t>
+  </si>
+  <si>
+    <t>bestanden</t>
+  </si>
+  <si>
+    <t>pruefungsfrei</t>
+  </si>
 </sst>
 </file>
 
@@ -203,12 +326,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -518,7 +644,7 @@
   <dimension ref="A1:U987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -620,27 +746,59 @@
         <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="2">
+        <v>2</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T2" s="2">
+        <v>18.8</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
@@ -652,24 +810,54 @@
       <c r="C3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="N3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T3" s="2">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
@@ -692,19 +880,45 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1001</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
@@ -727,44 +941,108 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1001</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T5" s="2">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="B6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2000</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
+      <c r="N6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T6" s="2">
+        <v>19.7</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
@@ -776,24 +1054,56 @@
       <c r="C7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="2">
+        <v>3000</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M7" s="2">
+        <v>2</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T7" s="2">
+        <v>18.8</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
@@ -805,24 +1115,56 @@
       <c r="C8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="2">
+        <v>3000</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M8" s="2">
+        <v>2</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
@@ -839,19 +1181,45 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="2">
+        <v>4000</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M9" s="2">
+        <v>2</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="T9" s="2">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
@@ -864,7 +1232,7 @@
         <v>38</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>42</v>
@@ -874,19 +1242,45 @@
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M10" s="2">
+        <v>2</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T10" s="2">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
@@ -909,19 +1303,43 @@
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" s="2">
+        <v>2000</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
+      <c r="N11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T11" s="2">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>

</xml_diff>